<commit_message>
Common: Preparing lab stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB0DFDC-1AAD-4DE9-BDCD-C09575738F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF783F8-80FB-42F7-AC50-EF1EC1973BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="3315" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="499">
   <si>
     <t>cs</t>
   </si>
@@ -431,6 +431,18 @@
     <t>Veřejný web</t>
   </si>
   <si>
+    <t>lab.home.title</t>
+  </si>
+  <si>
+    <t>lab.build.menu</t>
+  </si>
+  <si>
+    <t>Buildy</t>
+  </si>
+  <si>
+    <t>lab.home.menu</t>
+  </si>
+  <si>
     <t>common.sign-out.tooltip</t>
   </si>
   <si>
@@ -725,6 +737,18 @@
     <t>Jméno</t>
   </si>
   <si>
+    <t>lab.home.subtitle</t>
+  </si>
+  <si>
+    <t>lab.vape.menu</t>
+  </si>
+  <si>
+    <t>lab.liquid.menu</t>
+  </si>
+  <si>
+    <t>Liquidy</t>
+  </si>
+  <si>
     <t>Atomizéry</t>
   </si>
   <si>
@@ -735,6 +759,9 @@
   </si>
   <si>
     <t>Vaty</t>
+  </si>
+  <si>
+    <t>Vape</t>
   </si>
   <si>
     <t>Báze</t>
@@ -1508,6 +1535,36 @@
   </si>
   <si>
     <t>lab.index.title</t>
+  </si>
+  <si>
+    <t>Vítejte v laboratoři; zda najdete veškeré nástroje užitečné pro sledování zrání liquidů, grafy vapů, evidence buildů a mnoho dalšího.</t>
+  </si>
+  <si>
+    <t>lab.inventory.menu</t>
+  </si>
+  <si>
+    <t>Inventář</t>
+  </si>
+  <si>
+    <t>lab.inventory.atomizer.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.aroma.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.booster.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.base.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.mod.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.cotton.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.cell.menu</t>
   </si>
 </sst>
 </file>
@@ -1572,13 +1629,16 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="import" xfId="2" xr:uid="{DD1BC027-BC6C-4B34-B536-A533FDE94B7A}"/>
@@ -1891,7 +1951,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1899,7 +1959,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1907,7 +1967,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1915,7 +1975,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1923,7 +1983,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1931,7 +1991,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1939,7 +1999,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1982,7 +2042,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1990,10 +2050,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2021,10 +2081,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2032,10 +2092,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2054,10 +2114,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2065,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2076,10 +2136,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2087,10 +2147,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2109,10 +2169,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2120,10 +2180,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2131,10 +2191,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,10 +2202,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2153,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2164,10 +2224,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2175,10 +2235,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,10 +2246,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -2197,10 +2257,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -2208,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2219,10 +2279,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2230,10 +2290,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2241,10 +2301,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2252,10 +2312,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -2263,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,10 +2334,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -2285,10 +2345,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2296,10 +2356,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2307,10 +2367,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,10 +2378,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,10 +2389,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2351,10 +2411,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2362,10 +2422,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2373,10 +2433,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2384,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>10</v>
@@ -2416,10 +2476,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2448,10 +2508,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2514,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -2525,10 +2585,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,10 +2596,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2547,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -2558,10 +2618,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2569,10 +2629,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2580,10 +2640,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2591,10 +2651,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,10 +2662,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -2613,10 +2673,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2624,10 +2684,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -2635,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2646,10 +2706,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="230.25" x14ac:dyDescent="0.25">
@@ -2657,10 +2717,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="102.75" x14ac:dyDescent="0.25">
@@ -2668,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="166.5" x14ac:dyDescent="0.25">
@@ -2679,10 +2739,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -2693,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,10 +2771,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2722,10 +2782,164 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2753,10 +2967,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2764,10 +2978,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2775,10 +2989,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2808,10 +3022,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2819,7 +3033,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
@@ -2830,10 +3044,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2841,10 +3055,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2852,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2863,10 +3077,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2907,10 +3121,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2918,10 +3132,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2940,10 +3154,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2951,10 +3165,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2962,10 +3176,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2973,10 +3187,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2984,10 +3198,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2995,10 +3209,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3006,10 +3220,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3028,10 +3242,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3039,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>22</v>
@@ -3050,10 +3264,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3061,10 +3275,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3072,10 +3286,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3083,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>72</v>
@@ -3149,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>27</v>
@@ -3237,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>27</v>
@@ -3248,10 +3462,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3259,10 +3473,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3270,10 +3484,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3281,10 +3495,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3336,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>30</v>
@@ -3347,10 +3561,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,10 +3572,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3369,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>59</v>
@@ -3380,10 +3594,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3391,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>59</v>
@@ -3468,10 +3682,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3479,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>110</v>
@@ -3490,10 +3704,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3501,10 +3715,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3512,10 +3726,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3523,10 +3737,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3534,10 +3748,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3545,10 +3759,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3556,10 +3770,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3567,10 +3781,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3589,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>59</v>
@@ -3600,10 +3814,10 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3611,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>112</v>
@@ -3622,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>116</v>
@@ -3633,10 +3847,10 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="82" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3644,10 +3858,10 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3655,10 +3869,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3666,10 +3880,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3677,10 +3891,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3688,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>30</v>
@@ -3699,10 +3913,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3710,10 +3924,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3721,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3732,10 +3946,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3743,10 +3957,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3754,10 +3968,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3765,10 +3979,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3776,10 +3990,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3787,10 +4001,10 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -3819,10 +4033,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3830,10 +4044,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3841,10 +4055,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,10 +4077,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,10 +4088,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,10 +4110,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,10 +4121,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3940,10 +4154,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3962,10 +4176,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3973,10 +4187,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3984,10 +4198,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3995,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>40</v>
@@ -4248,7 +4462,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>30</v>
@@ -4259,7 +4473,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>75</v>
@@ -4270,10 +4484,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4281,10 +4495,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4292,10 +4506,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4303,10 +4517,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4314,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>65</v>
@@ -4325,10 +4539,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4336,10 +4550,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4347,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>68</v>
@@ -4358,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>63</v>
@@ -4369,10 +4583,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4380,7 +4594,7 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
@@ -4391,7 +4605,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>100</v>
@@ -4402,10 +4616,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4413,10 +4627,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4424,10 +4638,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4435,10 +4649,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4446,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>30</v>
@@ -4457,10 +4671,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -4488,10 +4702,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4499,10 +4713,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4510,10 +4724,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4521,7 +4735,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -4532,7 +4746,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>126</v>
@@ -4543,10 +4757,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4554,10 +4768,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4565,10 +4779,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4576,10 +4790,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4587,10 +4801,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4598,10 +4812,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4609,10 +4823,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4620,10 +4834,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4631,10 +4845,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4642,10 +4856,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4653,10 +4867,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4664,10 +4878,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -4675,10 +4889,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4686,10 +4900,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4697,10 +4911,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4708,10 +4922,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4719,10 +4933,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4730,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4741,10 +4955,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -4752,10 +4966,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4763,10 +4977,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -4774,10 +4988,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -4785,10 +4999,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -4796,10 +5010,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -4807,10 +5021,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4818,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4829,10 +5043,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -4840,10 +5054,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -4851,10 +5065,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4862,10 +5076,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4873,10 +5087,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4884,10 +5098,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4895,10 +5109,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -4906,10 +5120,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4917,10 +5131,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4928,10 +5142,10 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4939,10 +5153,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4950,10 +5164,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4961,10 +5175,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4972,10 +5186,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4983,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4994,10 +5208,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -5005,10 +5219,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -5016,10 +5230,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -5027,10 +5241,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -5038,10 +5252,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -5049,10 +5263,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -5060,10 +5274,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5071,10 +5285,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -5082,10 +5296,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: So, it's quite cool now!
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF783F8-80FB-42F7-AC50-EF1EC1973BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E19F66-DE71-47C4-B04A-E6723349DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3315" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="501">
   <si>
     <t>cs</t>
   </si>
@@ -1565,6 +1565,12 @@
   </si>
   <si>
     <t>lab.inventory.cell.menu</t>
+  </si>
+  <si>
+    <t>Správa aplikace</t>
+  </si>
+  <si>
+    <t>lab.root.home.menu</t>
   </si>
 </sst>
 </file>
@@ -2753,10 +2759,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2940,6 +2946,17 @@
       </c>
       <c r="C16" s="1" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Another set of boirelplate shits
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E19F66-DE71-47C4-B04A-E6723349DBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C29F34-F268-42E6-90CE-9116728D1DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="3315" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="508">
   <si>
     <t>cs</t>
   </si>
@@ -1571,6 +1571,27 @@
   </si>
   <si>
     <t>lab.root.home.menu</t>
+  </si>
+  <si>
+    <t>lab.inventory.atomizer.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.mod.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.cell.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.cotton.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.aroma.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.base.index.title</t>
+  </si>
+  <si>
+    <t>lab.inventory.booster.index.title</t>
   </si>
 </sst>
 </file>
@@ -2759,10 +2780,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,6 +2978,83 @@
       </c>
       <c r="C17" s="1" t="s">
         <v>499</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added email login support
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B4F00E-8FBC-4BCF-9D5B-0BF2E00CA4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F7041-011A-4D4D-B32F-D656DB37CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="533">
   <si>
     <t>cs</t>
   </si>
@@ -1658,6 +1658,18 @@
   </si>
   <si>
     <t>lab.cell.inventory.menu</t>
+  </si>
+  <si>
+    <t>public.sign-in.email.button</t>
+  </si>
+  <si>
+    <t>Přihlásit se</t>
+  </si>
+  <si>
+    <t>Zadejte prosím svůj email</t>
+  </si>
+  <si>
+    <t>public.sign-in.email.label.required</t>
   </si>
 </sst>
 </file>
@@ -2583,10 +2595,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC49E62-0AEE-40E6-B00F-514263105890}">
-  <dimension ref="A1:C22"/>
+  <sheetPr codeName="List1"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,6 +2851,28 @@
         <v>373</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2848,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Added initial inventory stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F7041-011A-4D4D-B32F-D656DB37CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE273BA-4271-4151-B29E-31C41F2688D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="534">
   <si>
     <t>cs</t>
   </si>
@@ -1670,6 +1670,9 @@
   </si>
   <si>
     <t>public.sign-in.email.label.required</t>
+  </si>
+  <si>
+    <t>lab.market.menu</t>
   </si>
 </sst>
 </file>
@@ -2598,8 +2601,8 @@
   <sheetPr codeName="List1"/>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4900,10 +4903,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5650,6 +5653,17 @@
         <v>514</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Added transaction to liquid
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE273BA-4271-4151-B29E-31C41F2688D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC22176-4FE3-47BE-BFE8-D72285D2E8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1095" yWindow="2160" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="535">
   <si>
     <t>cs</t>
   </si>
@@ -1673,6 +1673,9 @@
   </si>
   <si>
     <t>lab.market.menu</t>
+  </si>
+  <si>
+    <t>lab.liquid.index.title</t>
   </si>
 </sst>
 </file>
@@ -4903,10 +4906,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5664,6 +5667,17 @@
         <v>341</v>
       </c>
     </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Improved amount display of transaction
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A2DD83-4CE2-46AB-92D7-19BB2E4850D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A0DF7-9C83-4329-9699-8A185E80A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="2490" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1681,9 +1681,6 @@
     <t>lab.liquid.create.success</t>
   </si>
   <si>
-    <t>Liquid [{{data.name}}] byl úspěšně vytvořen za {{data.transaction.amount}} puffíků.</t>
-  </si>
-  <si>
     <t>lab.liquid.create.title</t>
   </si>
   <si>
@@ -1709,6 +1706,9 @@
   </si>
   <si>
     <t>Uložit</t>
+  </si>
+  <si>
+    <t>Liquid [{{data.name}}] byl úspěšně vytvořen za {{data.amount}} puffíků.</t>
   </si>
 </sst>
 </file>
@@ -2923,7 +2923,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3227,7 +3227,7 @@
         <v>535</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3235,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>186</v>
@@ -3257,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3268,10 +3268,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3279,10 +3279,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>544</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A little nice improvement
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A0DF7-9C83-4329-9699-8A185E80A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F207427-1122-4E5F-9E2E-63511BFD83D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2490" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="2550" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="548">
   <si>
     <t>cs</t>
   </si>
@@ -1709,6 +1709,12 @@
   </si>
   <si>
     <t>Liquid [{{data.name}}] byl úspěšně vytvořen za {{data.amount}} puffíků.</t>
+  </si>
+  <si>
+    <t>common.job.all.done</t>
+  </si>
+  <si>
+    <t>Všechny úlohy jsou dokončené.</t>
   </si>
 </sst>
 </file>
@@ -2207,10 +2213,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,6 +2598,17 @@
       </c>
       <c r="C34" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -2922,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,6 +3304,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3294,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Some quite nice stuff there
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9251701-2C5F-4CE8-B449-C6B542C28DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F6B6FC-5C8E-4987-AFC0-25DBBC4DF478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2550" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="1545" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="554">
   <si>
     <t>cs</t>
   </si>
@@ -1684,9 +1684,6 @@
     <t>lab.liquid.create.title</t>
   </si>
   <si>
-    <t>Nový liquid</t>
-  </si>
-  <si>
     <t>lab.liquid.name.label</t>
   </si>
   <si>
@@ -1727,6 +1724,15 @@
   </si>
   <si>
     <t>Přidám liquidu si jej zaevidujete a můžete sledovat různé zajímavé hodnoty, jako jsou například datum jeho dozrání, datum expirace (pokud to stihne) nebo vypočtené poměry PG/VG.</t>
+  </si>
+  <si>
+    <t>error.Not enough puffies</t>
+  </si>
+  <si>
+    <t>Omlouváme se, ale na tuto akci nemáte dostatek puffíků.</t>
+  </si>
+  <si>
+    <t>Nový liquid ({{data.price}} puffíků)</t>
   </si>
 </sst>
 </file>
@@ -2617,10 +2623,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +2640,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2661,17 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2952,7 +2968,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3256,7 +3272,7 @@
         <v>535</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3267,7 +3283,7 @@
         <v>536</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>537</v>
+        <v>553</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3275,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>186</v>
@@ -3286,10 +3302,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3297,10 +3313,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,10 +3324,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,10 +3335,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3330,10 +3346,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite interesting stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F6B6FC-5C8E-4987-AFC0-25DBBC4DF478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9982E4C2-A7D3-4943-BC1A-F99F7496D582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1545" yWindow="1545" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="560">
   <si>
     <t>cs</t>
   </si>
@@ -1733,6 +1733,24 @@
   </si>
   <si>
     <t>Nový liquid ({{data.price}} puffíků)</t>
+  </si>
+  <si>
+    <t>lab.aroma.list.empty.title</t>
+  </si>
+  <si>
+    <t>Nemáte koupená žádná aromata.</t>
+  </si>
+  <si>
+    <t>lab.aroma.list.empty.subtitle</t>
+  </si>
+  <si>
+    <t>lab.aroma.purchase.button</t>
+  </si>
+  <si>
+    <t>Přejít aromata</t>
+  </si>
+  <si>
+    <t>Pro tvorbu liquidu je zapotřebí mít jej z čeho vytvořit, tudíž je potřeba si pořídit nějaké aroma (do této kategorie spadají i již hotové liquidy).</t>
   </si>
 </sst>
 </file>
@@ -2965,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3350,6 +3368,39 @@
       </c>
       <c r="C34" s="1" t="s">
         <v>550</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: A little refactor to simplify repository stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA7B0B7-08BB-4E5E-A906-F5BED0140BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A47C73-110D-439F-A5EA-F26C1720E200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="1545" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="1605" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="571">
   <si>
     <t>cs</t>
   </si>
@@ -1732,9 +1732,6 @@
     <t>Omlouváme se, ale na tuto akci nemáte dostatek puffíků.</t>
   </si>
   <si>
-    <t>Nový liquid ({{data.price}} puffíků)</t>
-  </si>
-  <si>
     <t>lab.aroma.list.empty.title</t>
   </si>
   <si>
@@ -1754,6 +1751,39 @@
   </si>
   <si>
     <t>common.loading</t>
+  </si>
+  <si>
+    <t>Nový liquid</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.wizard.tab</t>
+  </si>
+  <si>
+    <t>Kouzelník</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.common.tab</t>
+  </si>
+  <si>
+    <t>Ruční zadání</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.simple.tab</t>
+  </si>
+  <si>
+    <t>Zrychlené zadání</t>
+  </si>
+  <si>
+    <t>lab.liquid.aromaId.label</t>
+  </si>
+  <si>
+    <t>Aroma</t>
+  </si>
+  <si>
+    <t>lab.liquid.aromaId.label.required</t>
+  </si>
+  <si>
+    <t>Vyberte prosím aroma (příchuť) liquidu.</t>
   </si>
 </sst>
 </file>
@@ -2254,8 +2284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2685,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>76</v>
@@ -2997,10 +3027,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3315,7 +3345,7 @@
         <v>536</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3389,10 +3419,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3400,10 +3430,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3411,10 +3441,65 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>558</v>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Quite nice stuff there!
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E915CE-30B1-4211-B687-3EA00201D015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0196B20F-31F0-471C-B115-5B5233E542DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="405" yWindow="1950" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="618">
   <si>
     <t>cs</t>
   </si>
@@ -1723,9 +1723,6 @@
     <t>lab.liquid.list.empty.subtitle</t>
   </si>
   <si>
-    <t>Přidám liquidu si jej zaevidujete a můžete sledovat různé zajímavé hodnoty, jako jsou například datum jeho dozrání, datum expirace (pokud to stihne) nebo vypočtené poměry PG/VG.</t>
-  </si>
-  <si>
     <t>error.Not enough puffies</t>
   </si>
   <si>
@@ -1864,15 +1861,9 @@
     <t>lab.liquid.preview.aroma.pgvg</t>
   </si>
   <si>
-    <t>Poměr PG/VG aromatu</t>
-  </si>
-  <si>
     <t>lab.liquid.preview.base.pgvg</t>
   </si>
   <si>
-    <t>Poměr PG/VG báze</t>
-  </si>
-  <si>
     <t>lab.liquid.preview.base.content</t>
   </si>
   <si>
@@ -1888,7 +1879,52 @@
     <t>lab.liquid.create.quick-mix.subtitle</t>
   </si>
   <si>
-    <t>Tato funkce umožní namíchání liquidu formou dolití bází, kdy už víte, co děláte a není třeba složitého vyklikávání dalších údajů. Touto cestou vzniknou beznikotinové liquidy.</t>
+    <t>lab.liquid.hint.vg.60</t>
+  </si>
+  <si>
+    <t>Poměrně běžný poměr který je spíše vhodný pro MTL vaping (tudíž je třeba mít patřičný build), případně pody, které tento poměr snesou. Celkový mix bude mírně hustější (díky trochu většímu množství VG).</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.50</t>
+  </si>
+  <si>
+    <t>Běžný poměr, který je relativně řídký, tudíž je vhodný do MTL (díky PG nese chuť), je ovšem třeba mít pro tento poměr správný build, protože může protékat.</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.30</t>
+  </si>
+  <si>
+    <t>Liquid vhodný pro MTL, může velmi dobře nést chuť, nicméně díky velkému poměru PG bude velmi řídký, tudíž s tím bude třeba počítat při buildu nebo použití v podu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.40</t>
+  </si>
+  <si>
+    <t>Tento poměr bude spíše tekutější (díky většímu poměru PG) a bude lépe nést chuť. Vhodnější do MTL s patřičným buildem (může protékat).</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.80</t>
+  </si>
+  <si>
+    <t>Jedná se o poměrně extrémní poměr více hrčen pro DL vapování, kde je potlačena chuť ve prospěch velkých mraků. Celkový mix bude hustý, proto je třeba s tímto faktem počítat v buildech (hustý liquid nemusí být schopný rychle zásobit vatu u spirálky).</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.70</t>
+  </si>
+  <si>
+    <t>Celkem oblíbený poměr spíše určený pro DL vaping, jelikož výsledná směs bude produkovat více páry na úkor chuti. Také se jedná o hustější liquid, tudíž je potřeba s tímto počítat u buildu.</t>
+  </si>
+  <si>
+    <t>Poměr VG/PG aromatu</t>
+  </si>
+  <si>
+    <t>Poměr VG/PG báze</t>
+  </si>
+  <si>
+    <t>Přidám liquidu si jej zaevidujete a můžete sledovat různé zajímavé hodnoty, jako jsou například datum jeho dozrání, datum expirace (pokud to stihne) nebo vypočtené poměry VG/PG.</t>
+  </si>
+  <si>
+    <t>Tato funkce umožní namíchání liquidu formou dolití bází, kdy už víte, co děláte a není třeba složitého vyklikávání dalších údajů.</t>
   </si>
 </sst>
 </file>
@@ -2790,7 +2826,7 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>76</v>
@@ -2801,10 +2837,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2812,10 +2848,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2823,10 +2859,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,10 +2870,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -2877,10 +2913,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -3176,10 +3212,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3205,21 +3241,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>488</v>
+        <v>524</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>126</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>126</v>
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3227,10 +3263,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>231</v>
+        <v>554</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>489</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3238,10 +3274,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>552</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3249,20 +3285,20 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>490</v>
+        <v>555</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>491</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3271,10 +3307,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>481</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3282,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>483</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3304,10 +3340,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>519</v>
+        <v>583</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>236</v>
+        <v>584</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3315,10 +3351,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>130</v>
+        <v>582</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>131</v>
+        <v>588</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3326,10 +3362,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>232</v>
+        <v>585</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>239</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3337,10 +3373,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>233</v>
+        <v>526</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>234</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3348,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>238</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3359,10 +3395,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>528</v>
+        <v>130</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>237</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3370,10 +3406,10 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>493</v>
+        <v>522</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>492</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3381,10 +3417,10 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3392,10 +3428,10 @@
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3403,10 +3439,10 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3414,21 +3450,21 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>523</v>
+        <v>132</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>524</v>
+        <v>231</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3436,10 +3472,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>525</v>
+        <v>129</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>240</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3447,10 +3483,10 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>526</v>
+        <v>488</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>483</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3458,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>533</v>
+        <v>490</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>341</v>
+        <v>491</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3469,10 +3505,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>534</v>
+        <v>563</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>234</v>
+        <v>564</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3480,10 +3516,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>535</v>
+        <v>565</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>544</v>
+        <v>566</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3491,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>536</v>
+        <v>574</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3502,10 +3538,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3513,10 +3549,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>538</v>
+        <v>589</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>539</v>
+        <v>590</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3524,10 +3560,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>540</v>
+        <v>576</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>541</v>
+        <v>577</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3546,10 +3582,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>548</v>
+        <v>572</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3557,10 +3593,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>549</v>
+        <v>601</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>550</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3568,21 +3604,21 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>553</v>
+        <v>599</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3590,10 +3626,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>587</v>
+        <v>544</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3601,10 +3637,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>560</v>
+        <v>536</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3612,76 +3648,76 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>563</v>
+        <v>606</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>564</v>
+        <v>608</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>566</v>
+        <v>604</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>574</v>
+        <v>602</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>575</v>
+        <v>612</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>577</v>
+        <v>610</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>578</v>
+        <v>611</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3689,21 +3725,21 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>583</v>
+        <v>534</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>584</v>
+        <v>549</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>585</v>
+        <v>616</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3711,10 +3747,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>586</v>
+        <v>547</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>588</v>
+        <v>548</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3722,10 +3758,10 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>590</v>
+        <v>233</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>591</v>
+        <v>234</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3733,10 +3769,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>592</v>
+        <v>540</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>593</v>
+        <v>541</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3744,10 +3780,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>594</v>
+        <v>537</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>595</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3755,10 +3791,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>597</v>
+        <v>614</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3766,10 +3802,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3777,10 +3813,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>601</v>
+        <v>615</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3788,24 +3824,93 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>605</v>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C62">
+    <sortCondition ref="B59:B62"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Preparing booster support
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC57F0E2-0A92-477D-B836-7298F28ABFC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA83739B-A128-46DB-A97B-ED9841783DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9180" yWindow="495" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="1785" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="628">
   <si>
     <t>cs</t>
   </si>
@@ -1931,6 +1931,30 @@
   </si>
   <si>
     <t>Poměr VG/PG</t>
+  </si>
+  <si>
+    <t>lab.liquid.boosterId.label</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>lab.liquid.boosterId.label.tooltip</t>
+  </si>
+  <si>
+    <t>Pokud si přejete přidat do liquidu nikotin, vyberte prosím booster a výslednou sílu nikotinu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.nicotine.label</t>
+  </si>
+  <si>
+    <t>Množství nikotinu</t>
+  </si>
+  <si>
+    <t>lab.liquid.nicotine.label.tooltip</t>
+  </si>
+  <si>
+    <t>Vyberte požadované množství nikotinu; je třeba mít správně vybraný booster nejen kvůli jeho síle, ale také kvůli poměru VG/PG, jelikož boosteru obvykle bývá větší množství a může výrazně pohnout s výsledným poměrem liquidu.</t>
   </si>
 </sst>
 </file>
@@ -3218,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3577,10 +3601,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>542</v>
+        <v>620</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>543</v>
+        <v>621</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3588,21 +3612,21 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>561</v>
+        <v>622</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>601</v>
+        <v>542</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>617</v>
+        <v>543</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3610,21 +3634,21 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>599</v>
+        <v>561</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>562</v>
+        <v>601</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>571</v>
+        <v>617</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3632,10 +3656,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>535</v>
+        <v>599</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>544</v>
+        <v>600</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3643,10 +3667,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>536</v>
+        <v>562</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>558</v>
+        <v>571</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,32 +3678,32 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>560</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3687,10 +3711,10 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3698,10 +3722,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>603</v>
+        <v>609</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3709,43 +3733,43 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="1" t="s">
+    <row r="47" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>611</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3753,21 +3777,21 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>233</v>
+        <v>549</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>234</v>
+        <v>616</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3775,10 +3799,10 @@
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3786,10 +3810,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>537</v>
+        <v>233</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3797,10 +3821,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>595</v>
+        <v>540</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>614</v>
+        <v>541</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,10 +3832,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>597</v>
+        <v>537</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>598</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3819,21 +3843,21 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>596</v>
+        <v>624</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>591</v>
+        <v>626</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>592</v>
+        <v>627</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3841,10 +3865,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>618</v>
+        <v>595</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3852,10 +3876,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3863,10 +3887,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>538</v>
+        <v>596</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>539</v>
+        <v>615</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3874,10 +3898,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>533</v>
+        <v>591</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>341</v>
+        <v>592</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,10 +3909,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>521</v>
+        <v>618</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>236</v>
+        <v>619</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3896,10 +3920,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>519</v>
+        <v>593</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>236</v>
+        <v>594</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,10 +3931,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>493</v>
+        <v>538</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>492</v>
+        <v>539</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3918,15 +3942,59 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C63">
-    <sortCondition ref="B57:B63"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C67">
+    <sortCondition ref="B63:B67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: A little refactor
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA83739B-A128-46DB-A97B-ED9841783DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A480D0DA-40D8-400C-B5A6-DF8E602575B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1530" yWindow="1785" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="630">
   <si>
     <t>cs</t>
   </si>
@@ -1955,6 +1955,12 @@
   </si>
   <si>
     <t>Vyberte požadované množství nikotinu; je třeba mít správně vybraný booster nejen kvůli jeho síle, ale také kvůli poměru VG/PG, jelikož boosteru obvykle bývá větší množství a může výrazně pohnout s výsledným poměrem liquidu.</t>
+  </si>
+  <si>
+    <t>lab.liquid.hint.vg.90</t>
+  </si>
+  <si>
+    <t>Extrémní mix zaměřený hlavně na DL, velmi hustý na úkor chuťového projevu. Build je třeba připravit na tento velmi hustý liquid.</t>
   </si>
 </sst>
 </file>
@@ -3242,10 +3248,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,37 +3778,37 @@
         <v>611</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3810,10 +3816,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>233</v>
+        <v>547</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>234</v>
+        <v>548</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3821,10 +3827,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>540</v>
+        <v>233</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>541</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -3832,10 +3838,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>186</v>
+        <v>541</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3843,32 +3849,32 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>627</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3876,10 +3882,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3887,10 +3893,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>615</v>
+        <v>598</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3898,10 +3904,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>592</v>
+        <v>615</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3909,10 +3915,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>618</v>
+        <v>591</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>619</v>
+        <v>592</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3920,10 +3926,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>593</v>
+        <v>618</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>594</v>
+        <v>619</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3931,10 +3937,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>538</v>
+        <v>593</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>539</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3942,10 +3948,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>341</v>
+        <v>539</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3953,10 +3959,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3970,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>236</v>
@@ -3975,10 +3981,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>493</v>
+        <v>519</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>492</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3986,15 +3992,26 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C67">
-    <sortCondition ref="B63:B67"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C68">
+    <sortCondition ref="B55:B68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Still working on booster stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A480D0DA-40D8-400C-B5A6-DF8E602575B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E3664F-E840-4582-8696-521619BA12A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1530" yWindow="1785" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="632">
   <si>
     <t>cs</t>
   </si>
@@ -1906,9 +1906,6 @@
     <t>lab.liquid.hint.vg.80</t>
   </si>
   <si>
-    <t>Jedná se o poměrně extrémní poměr více hrčen pro DL vapování, kde je potlačena chuť ve prospěch velkých mraků. Celkový mix bude hustý, proto je třeba s tímto faktem počítat v buildech (hustý liquid nemusí být schopný rychle zásobit vatu u spirálky).</t>
-  </si>
-  <si>
     <t>lab.liquid.hint.vg.70</t>
   </si>
   <si>
@@ -1961,6 +1958,15 @@
   </si>
   <si>
     <t>Extrémní mix zaměřený hlavně na DL, velmi hustý na úkor chuťového projevu. Build je třeba připravit na tento velmi hustý liquid.</t>
+  </si>
+  <si>
+    <t>Jedná se o poměrně extrémní poměr více určen pro DL vapování, kde je potlačena chuť ve prospěch velkých mraků. Celkový mix bude hustý, proto je třeba s tímto faktem počítat v buildech (hustý liquid nemusí být schopný rychle zásobit vatu u spirálky).</t>
+  </si>
+  <si>
+    <t>lab.liquid.preview.booster.content</t>
+  </si>
+  <si>
+    <t>Množství boosteru</t>
   </si>
 </sst>
 </file>
@@ -3248,10 +3254,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3607,10 +3613,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3618,10 +3624,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3654,7 +3660,7 @@
         <v>601</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3761,10 +3767,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>612</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -3775,7 +3781,7 @@
         <v>610</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>611</v>
+        <v>629</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3783,10 +3789,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3808,7 +3814,7 @@
         <v>549</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,10 +3866,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="39" x14ac:dyDescent="0.25">
@@ -3871,10 +3877,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3891,7 @@
         <v>595</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3907,7 +3913,7 @@
         <v>596</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3915,10 +3921,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>591</v>
+        <v>630</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>592</v>
+        <v>631</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3926,10 +3932,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>618</v>
+        <v>591</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>619</v>
+        <v>592</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3937,10 +3943,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>593</v>
+        <v>617</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>594</v>
+        <v>618</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3948,10 +3954,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>538</v>
+        <v>593</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>539</v>
+        <v>594</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3959,10 +3965,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>341</v>
+        <v>539</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3970,10 +3976,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3981,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>236</v>
@@ -3992,10 +3998,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>493</v>
+        <v>519</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>492</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4003,15 +4009,26 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C68">
-    <sortCondition ref="B55:B68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C69">
+    <sortCondition ref="B60:B69"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Trying to improve the stuff
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869A384-DBDA-4BEB-9FD3-52BEAFB918A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B80B69-0AAC-4C12-BAF1-4DFFBFFE990D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="1785" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11145" yWindow="2325" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="644">
   <si>
     <t>cs</t>
   </si>
@@ -1750,18 +1750,6 @@
     <t>Nový liquid</t>
   </si>
   <si>
-    <t>lab.liquid.create.wizard.tab</t>
-  </si>
-  <si>
-    <t>Kouzelník</t>
-  </si>
-  <si>
-    <t>lab.liquid.create.common.tab</t>
-  </si>
-  <si>
-    <t>lab.liquid.create.simple.tab</t>
-  </si>
-  <si>
     <t>lab.liquid.aromaId.label</t>
   </si>
   <si>
@@ -1789,9 +1777,6 @@
     <t>QuickMix</t>
   </si>
   <si>
-    <t>SlowMix</t>
-  </si>
-  <si>
     <t>lab.liquid.baseId.label</t>
   </si>
   <si>
@@ -2009,6 +1994,15 @@
   </si>
   <si>
     <t>Zkontrolovat</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.quick-mix.tab</t>
+  </si>
+  <si>
+    <t>lab.liquid.create.advanced.tab</t>
+  </si>
+  <si>
+    <t>Pokročilé</t>
   </si>
 </sst>
 </file>
@@ -2921,10 +2915,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2932,10 +2926,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2943,10 +2937,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2954,10 +2948,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -3296,10 +3290,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3372,7 +3366,7 @@
         <v>555</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3424,10 +3418,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3435,10 +3429,10 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3446,10 +3440,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3589,10 +3583,10 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3600,10 +3594,10 @@
         <v>0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3611,10 +3605,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3622,7 +3616,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>240</v>
@@ -3633,10 +3627,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3644,10 +3638,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3655,10 +3649,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3666,10 +3660,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3677,10 +3671,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3699,10 +3693,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>561</v>
+        <v>642</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>572</v>
+        <v>643</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3710,10 +3704,10 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3721,10 +3715,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3732,10 +3726,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>562</v>
+        <v>641</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3760,15 +3754,15 @@
         <v>558</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>559</v>
+        <v>631</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>560</v>
+        <v>632</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3776,10 +3770,10 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3787,10 +3781,10 @@
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>638</v>
+        <v>601</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>643</v>
+        <v>602</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3798,10 +3792,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3809,10 +3803,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3820,10 +3814,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -3831,65 +3825,65 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>615</v>
+        <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3897,10 +3891,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>547</v>
+        <v>233</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>548</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3908,10 +3902,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>233</v>
+        <v>540</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>234</v>
+        <v>541</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3919,10 +3913,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>540</v>
+        <v>639</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>541</v>
+        <v>640</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3930,10 +3924,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>644</v>
+        <v>537</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>645</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3941,32 +3935,32 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>537</v>
+        <v>618</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>625</v>
+        <v>590</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>626</v>
+        <v>608</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3974,10 +3968,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>613</v>
+        <v>593</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3985,10 +3979,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>598</v>
+        <v>609</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3996,10 +3990,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>614</v>
+        <v>626</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4007,10 +4001,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4018,10 +4012,10 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>632</v>
+        <v>586</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>633</v>
+        <v>587</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -4029,10 +4023,10 @@
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>591</v>
+        <v>629</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>592</v>
+        <v>630</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4051,10 +4045,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>639</v>
+        <v>612</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>640</v>
+        <v>613</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4062,10 +4056,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>617</v>
+        <v>588</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>618</v>
+        <v>589</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4073,10 +4067,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>593</v>
+        <v>538</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>594</v>
+        <v>539</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4084,10 +4078,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>539</v>
+        <v>341</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4095,10 +4089,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>341</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4106,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>236</v>
@@ -4117,10 +4111,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>519</v>
+        <v>493</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>236</v>
+        <v>492</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4128,26 +4122,15 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>493</v>
+        <v>232</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C76" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
-    <sortCondition ref="B73:B76"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
+    <sortCondition ref="B72:B75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Liquid stuff works quite well
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B80B69-0AAC-4C12-BAF1-4DFFBFFE990D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9A8F5-D378-4C01-A951-45D5433EB78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="2325" windowWidth="23610" windowHeight="18390" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11145" yWindow="2325" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="646">
   <si>
     <t>cs</t>
   </si>
@@ -2003,6 +2003,12 @@
   </si>
   <si>
     <t>Pokročilé</t>
+  </si>
+  <si>
+    <t>root.transaction.amount.label.required</t>
+  </si>
+  <si>
+    <t>Částka transakce je povinná.</t>
   </si>
 </sst>
 </file>
@@ -3292,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4139,10 +4145,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4377,10 +4383,10 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>226</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -4388,10 +4394,10 @@
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -4399,10 +4405,10 @@
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -4410,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>215</v>
@@ -4421,32 +4427,32 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -4454,10 +4460,10 @@
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>290</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -4465,10 +4471,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -4476,10 +4482,10 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4487,10 +4493,10 @@
         <v>0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4498,10 +4504,10 @@
         <v>0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>284</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4509,10 +4515,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -4520,10 +4526,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4531,10 +4537,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4542,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4553,7 +4559,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>291</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>27</v>
@@ -4564,10 +4570,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>291</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4575,10 +4581,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>363</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4586,10 +4592,10 @@
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>106</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4597,21 +4603,21 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4619,21 +4625,21 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4641,10 +4647,10 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>277</v>
+        <v>35</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4652,10 +4658,10 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>278</v>
+        <v>39</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>279</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4663,10 +4669,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>281</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4674,10 +4680,10 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4685,21 +4691,21 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>287</v>
+        <v>324</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>32</v>
+        <v>361</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>33</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4707,10 +4713,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>34</v>
+        <v>280</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>33</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4718,10 +4724,10 @@
         <v>0</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>21</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4729,10 +4735,10 @@
         <v>0</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>107</v>
+        <v>287</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>59</v>
+        <v>283</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4740,10 +4746,10 @@
         <v>0</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>195</v>
+        <v>32</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -4751,10 +4757,10 @@
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>194</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -4762,10 +4768,10 @@
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>191</v>
+        <v>20</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4773,7 +4779,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>59</v>
@@ -4784,10 +4790,10 @@
         <v>0</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4795,10 +4801,10 @@
         <v>0</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>292</v>
+        <v>193</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>59</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4806,10 +4812,10 @@
         <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>191</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4817,10 +4823,10 @@
         <v>0</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -4828,10 +4834,10 @@
         <v>0</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4839,10 +4845,10 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>24</v>
+        <v>292</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4850,10 +4856,10 @@
         <v>0</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>117</v>
+        <v>302</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4861,21 +4867,21 @@
         <v>0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>174</v>
+        <v>340</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>175</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4883,10 +4889,10 @@
         <v>0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>173</v>
+        <v>113</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4894,10 +4900,10 @@
         <v>0</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4905,10 +4911,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>179</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4916,10 +4922,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>190</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4927,10 +4933,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>176</v>
+        <v>411</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>177</v>
+        <v>412</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4938,10 +4944,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>187</v>
+        <v>644</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>188</v>
+        <v>645</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4949,10 +4955,10 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>181</v>
+        <v>413</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>182</v>
+        <v>414</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -4960,10 +4966,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>185</v>
+        <v>417</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>186</v>
+        <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4971,10 +4977,10 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>183</v>
+        <v>407</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>184</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4982,10 +4988,10 @@
         <v>0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>115</v>
+        <v>415</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>116</v>
+        <v>416</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4993,10 +4999,10 @@
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>302</v>
+        <v>409</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>59</v>
+        <v>410</v>
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -5004,21 +5010,21 @@
         <v>0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>324</v>
+        <v>109</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>336</v>
+        <v>174</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -5026,10 +5032,10 @@
         <v>0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>337</v>
+        <v>173</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -5037,21 +5043,21 @@
         <v>0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>340</v>
+        <v>178</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>361</v>
+        <v>180</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>362</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:3" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -5059,10 +5065,10 @@
         <v>0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>363</v>
+        <v>189</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>364</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,10 +5076,10 @@
         <v>0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>397</v>
+        <v>176</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>398</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -5081,10 +5087,10 @@
         <v>0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>399</v>
+        <v>187</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>401</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -5092,10 +5098,10 @@
         <v>0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>400</v>
+        <v>181</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>30</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -5103,10 +5109,10 @@
         <v>0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>402</v>
+        <v>185</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -5114,10 +5120,10 @@
         <v>0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>403</v>
+        <v>183</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>404</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -5125,10 +5131,10 @@
         <v>0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>406</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -5136,10 +5142,10 @@
         <v>0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -5147,10 +5153,10 @@
         <v>0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -5158,10 +5164,10 @@
         <v>0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>411</v>
+        <v>115</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>412</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -5169,10 +5175,10 @@
         <v>0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -5180,10 +5186,10 @@
         <v>0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>416</v>
+        <v>230</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -5191,13 +5197,27 @@
         <v>0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>417</v>
+        <v>337</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>418</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
+    <sortCondition ref="B87:B96"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: So, liquid stuff works quite nice now
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F9A8F5-D378-4C01-A951-45D5433EB78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B7474C-2EBD-4B19-927E-BB399BDE3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11145" yWindow="2325" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1260" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="648">
   <si>
     <t>cs</t>
   </si>
@@ -2009,6 +2009,12 @@
   </si>
   <si>
     <t>Částka transakce je povinná.</t>
+  </si>
+  <si>
+    <t>lab.liquid.quick-mix.success</t>
+  </si>
+  <si>
+    <t>Úspěšně jste si namíchali liquid [{{data.name}}].</t>
   </si>
 </sst>
 </file>
@@ -3296,10 +3302,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,10 +3727,10 @@
         <v>0</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>594</v>
+        <v>641</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3732,10 +3738,10 @@
         <v>0</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>641</v>
+        <v>594</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>567</v>
+        <v>595</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4073,10 +4079,10 @@
         <v>0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>538</v>
+        <v>646</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>539</v>
+        <v>647</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4084,10 +4090,10 @@
         <v>0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>341</v>
+        <v>539</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4095,10 +4101,10 @@
         <v>0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>236</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4106,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>236</v>
@@ -4117,10 +4123,10 @@
         <v>0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>493</v>
+        <v>519</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>492</v>
+        <v>236</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4128,15 +4134,26 @@
         <v>0</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C75">
-    <sortCondition ref="B72:B75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C76">
+    <sortCondition ref="B71:B76"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4147,8 +4164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17153922-55B5-46AD-9C90-5ED46DB8719C}">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Common: Added simple filter for boosters
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B7474C-2EBD-4B19-927E-BB399BDE3C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE9FA31-A4BB-4120-AC38-C119FF5944E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1260" windowWidth="23610" windowHeight="18390" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="1470" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="654">
   <si>
     <t>cs</t>
   </si>
@@ -2015,6 +2015,24 @@
   </si>
   <si>
     <t>Úspěšně jste si namíchali liquid [{{data.name}}].</t>
+  </si>
+  <si>
+    <t>common.quick-filter.label</t>
+  </si>
+  <si>
+    <t>Rychlý filtr</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.label</t>
+  </si>
+  <si>
+    <t>VG/PG</t>
+  </si>
+  <si>
+    <t>market.filter.nicotine.label</t>
+  </si>
+  <si>
+    <t>Nikotin</t>
   </si>
 </sst>
 </file>
@@ -2513,10 +2531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FA010E-31BE-4B9A-96A2-5C191961F568}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,6 +2982,17 @@
       </c>
       <c r="C40" s="1" t="s">
         <v>576</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -3304,7 +3333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01802250-F0AD-4E06-AE6E-C6C61B4E8147}">
   <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -5911,10 +5940,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6661,6 +6690,28 @@
         <v>514</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Common: Improved quick filters
</commit_message>
<xml_diff>
--- a/fixtures/00 - translations.xlsx
+++ b/fixtures/00 - translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152EDA34-6801-401B-B43C-24C0FD6582C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ADC029-588F-4B7D-ABED-7D7579CAA60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2535" yWindow="1470" windowWidth="23610" windowHeight="18390" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="657">
   <si>
     <t>cs</t>
   </si>
@@ -2033,6 +2033,15 @@
   </si>
   <si>
     <t>Nikotin</t>
+  </si>
+  <si>
+    <t>market.filter.pgvg.off.label</t>
+  </si>
+  <si>
+    <t>Vše</t>
+  </si>
+  <si>
+    <t>market.filter.nicotine.off.label</t>
   </si>
 </sst>
 </file>
@@ -5940,10 +5949,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97035108-4AB1-49C8-9E4F-911A1C9E966B}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6712,6 +6721,28 @@
         <v>653</v>
       </c>
     </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>